<commit_message>
complete task 41 & up to task 48
</commit_message>
<xml_diff>
--- a/docs/Agile-Product-Backlog.xlsx
+++ b/docs/Agile-Product-Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Programming Experiments\ASP.NET CORE\Pitcher\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Programming Experiments\ASP.NET CORE\Pitcher\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AC93DF-0991-4DC6-B695-19B90386669B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AD1C19-AEA2-471F-8F3D-2B2724959818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,7 +534,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -556,12 +556,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -696,16 +690,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="14" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -1056,8 +1050,8 @@
   <dimension ref="B1:AI106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K76" sqref="K76"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3608,34 +3602,34 @@
       <c r="AI49" s="3"/>
     </row>
     <row r="50" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="24">
+      <c r="B50" s="22">
         <v>34</v>
       </c>
-      <c r="C50" s="24" t="s">
+      <c r="C50" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="D50" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="E50" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="F50" s="25">
+      <c r="D50" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="23">
         <v>43938</v>
       </c>
-      <c r="G50" s="25">
+      <c r="G50" s="23">
         <v>44094</v>
       </c>
-      <c r="H50" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="I50" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J50" s="24">
+      <c r="H50" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J50" s="22">
         <v>20</v>
       </c>
-      <c r="K50" s="24"/>
+      <c r="K50" s="22"/>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
@@ -4188,34 +4182,34 @@
       <c r="AI60" s="3"/>
     </row>
     <row r="61" spans="2:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="22">
+      <c r="B61" s="24">
         <v>41</v>
       </c>
-      <c r="C61" s="22" t="s">
+      <c r="C61" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="D61" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E61" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="F61" s="23">
+      <c r="D61" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E61" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F61" s="25">
         <v>43967</v>
       </c>
-      <c r="G61" s="23">
+      <c r="G61" s="25">
         <v>43970</v>
       </c>
-      <c r="H61" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I61" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="J61" s="22">
+      <c r="H61" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I61" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="J61" s="24">
         <v>40</v>
       </c>
-      <c r="K61" s="22"/>
+      <c r="K61" s="24"/>
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
       <c r="N61" s="3"/>

</xml_diff>